<commit_message>
Se termina la implementación de la ruleta
</commit_message>
<xml_diff>
--- a/Ruleta.xlsx
+++ b/Ruleta.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jean\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\xampp\AMIN\Códigos\AMIN-Tarea1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A4D295-1918-4963-BB67-B158BE4CD4BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B07BB43-3A88-4140-A084-FE413EDA120F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
   <si>
     <t>Fitness</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Individuos - Tableros</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -127,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -141,6 +144,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1260,10 +1267,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:H11"/>
+  <dimension ref="B2:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,7 +1280,7 @@
     <col min="13" max="13" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1292,11 +1299,14 @@
       <c r="G2" s="8">
         <v>5</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="9" t="s">
         <v>1</v>
       </c>
+      <c r="I2" s="10" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1315,12 +1325,15 @@
       <c r="G3" s="1">
         <v>4</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <f>SUM(C3:G3)</f>
         <v>14</v>
       </c>
+      <c r="I3" s="1">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>2</v>
       </c>
@@ -1345,7 +1358,7 @@
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1370,7 +1383,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
@@ -1393,83 +1406,83 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="1">
-        <f>H3-C3</f>
-        <v>12</v>
+        <f>$I$3-C3</f>
+        <v>8</v>
       </c>
       <c r="D9" s="1">
-        <f>H3-D3</f>
-        <v>12</v>
+        <f t="shared" ref="D9:G9" si="1">$I$3-D3</f>
+        <v>8</v>
       </c>
       <c r="E9" s="1">
-        <f>H3-E3</f>
-        <v>12</v>
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
       <c r="F9" s="1">
-        <f>H3-F3</f>
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="G9" s="1">
-        <f>H3-G3</f>
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="H9" s="3">
         <f>SUM(C9:G9)</f>
-        <v>56</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="6">
         <f>C9/H9</f>
-        <v>0.21428571428571427</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="D10" s="6">
         <f>D9/H9</f>
-        <v>0.21428571428571427</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="E10" s="6">
         <f>E9/H9</f>
-        <v>0.21428571428571427</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="F10" s="6">
         <f>F9/H9</f>
-        <v>0.17857142857142858</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="G10" s="6">
         <f>G9/H9</f>
-        <v>0.17857142857142858</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="4">
         <f>C10</f>
-        <v>0.21428571428571427</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="D11" s="4">
         <f>C11+D10</f>
-        <v>0.42857142857142855</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="E11" s="4">
         <f>D11+E10</f>
-        <v>0.64285714285714279</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F11" s="4">
         <f>E11+F10</f>
-        <v>0.8214285714285714</v>
+        <v>0.83333333333333326</v>
       </c>
       <c r="G11" s="4">
         <f>F11+G10</f>
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
     </row>
   </sheetData>

</xml_diff>